<commit_message>
24.04.19 10:39PM Last Sales Details Updated
</commit_message>
<xml_diff>
--- a/Othes/Available Color For 23th april-.xlsx
+++ b/Othes/Available Color For 23th april-.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahbub.jamil\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">color!$A$1:$L$80</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -264,8 +259,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -391,7 +386,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,7 +421,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -603,417 +598,417 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="20.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="20.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="20.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="20.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="20.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="20.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="20.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="20.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="20.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="20.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="20.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="20.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="20.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="20.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="20.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="20.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="20.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="20.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="20.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="20.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="20.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="20.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="20.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="20.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="20.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="20.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="20.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="20.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="20.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="20.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="20.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="20.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="20.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="20.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="20.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="20.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="20.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="20.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="20.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="20.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="20.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="20.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="20.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="20.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="20.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="20.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" ht="20.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" ht="20.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" ht="20.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="20.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="20.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="20.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" ht="20.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="20.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="20.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" ht="20.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" ht="20.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" ht="20.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" ht="20.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="20.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="20.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" ht="20.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" ht="20.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" ht="20.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="20.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" ht="20.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" ht="20.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" ht="20.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="20.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" ht="20.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" ht="20.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" ht="20.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" ht="20.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" ht="20.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" ht="20.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" ht="20.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" ht="20.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" ht="20.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>